<commit_message>
added docstrings, modified tutorial, and updated parameters
</commit_message>
<xml_diff>
--- a/CRSP_ETC09132023.xlsx
+++ b/CRSP_ETC09132023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earleyn138/Library/CloudStorage/Box-Box/cryoscope/projects/etc/cryoscope_etc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earleyn138/research/PycharmProjects/cryoscope/cryoscope_etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971D1D27-B054-D04B-AFCA-C7B48B2A8107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C60F19-61CC-5D44-9EF6-F542F502E47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="500" windowWidth="27640" windowHeight="15940" activeTab="1" xr2:uid="{BB288948-5939-FC46-83E2-B7EB5588CFC4}"/>
+    <workbookView xWindow="10040" yWindow="1980" windowWidth="27640" windowHeight="15940" xr2:uid="{BB288948-5939-FC46-83E2-B7EB5588CFC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Prototype" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>Number of pixels on edge</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Effective number of pixels</t>
   </si>
   <si>
-    <t>Sky noise (e/s)</t>
-  </si>
-  <si>
     <t>Source rate (e/s)</t>
   </si>
   <si>
@@ -241,6 +238,12 @@
   </si>
   <si>
     <t>Measured from design, includes detector housing+spider vanes in FOV</t>
+  </si>
+  <si>
+    <t>Sky rate (e/s/pix)</t>
+  </si>
+  <si>
+    <t>Sky rate (e/s)</t>
   </si>
 </sst>
 </file>
@@ -349,15 +352,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,9 +445,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -482,7 +485,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -588,7 +591,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -730,7 +733,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -740,7 +743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEF58DD-D1C8-CB4C-8296-CC22CADB6B09}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -753,16 +758,16 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -770,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>5</v>
@@ -778,7 +783,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -831,7 +836,7 @@
         <v>4096</v>
       </c>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -890,7 +895,7 @@
         <v>8192</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -901,25 +906,25 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
@@ -937,51 +942,51 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" ref="F7:Q7" si="8">($E$7*F$5)/SQRT($E$7*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>282.4906665577098</v>
+        <v>282.82787412425989</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="8"/>
-        <v>399.5021318897289</v>
+        <v>399.97901540367889</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="8"/>
-        <v>564.9813331154196</v>
+        <v>565.65574824851979</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="8"/>
-        <v>799.0042637794578</v>
+        <v>799.95803080735777</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="8"/>
-        <v>1129.9626662308392</v>
+        <v>1131.3114964970396</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="8"/>
-        <v>1598.0085275589156</v>
+        <v>1599.9160616147155</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>2259.9253324616784</v>
+        <v>2262.6229929940791</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="8"/>
-        <v>3196.0170551178312</v>
+        <v>3199.8321232294311</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="8"/>
-        <v>4519.8506649233568</v>
+        <v>4525.2459859881583</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="8"/>
-        <v>6392.0341102356624</v>
+        <v>6399.6642464588622</v>
       </c>
       <c r="P7" s="5">
         <f t="shared" si="8"/>
-        <v>9039.7013298467136</v>
+        <v>9050.4919719763166</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="8"/>
-        <v>12784.068220471325</v>
+        <v>12799.328492917724</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -989,7 +994,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="1">
         <v>11</v>
@@ -1000,51 +1005,51 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" ref="F8:Q8" si="10">($E$8*F$5)/SQRT($E$8*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>175.10476423422216</v>
+        <v>175.61279338663738</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="10"/>
-        <v>247.63553241618024</v>
+        <v>248.35399413360676</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="10"/>
-        <v>350.20952846844432</v>
+        <v>351.22558677327476</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="10"/>
-        <v>495.27106483236048</v>
+        <v>496.70798826721352</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="10"/>
-        <v>700.41905693688864</v>
+        <v>702.45117354654951</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="10"/>
-        <v>990.54212966472096</v>
+        <v>993.41597653442705</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="10"/>
-        <v>1400.8381138737773</v>
+        <v>1404.902347093099</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="10"/>
-        <v>1981.0842593294419</v>
+        <v>1986.8319530688541</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="10"/>
-        <v>2801.6762277475545</v>
+        <v>2809.804694186198</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="10"/>
-        <v>3962.1685186588838</v>
+        <v>3973.6639061377082</v>
       </c>
       <c r="P8" s="5">
         <f t="shared" si="10"/>
-        <v>5603.3524554951091</v>
+        <v>5619.6093883723961</v>
       </c>
       <c r="Q8" s="5">
         <f t="shared" si="10"/>
-        <v>7924.3370373177677</v>
+        <v>7947.3278122754164</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -1063,51 +1068,51 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" ref="F9:Q9" si="11">($E$9*F$5)/SQRT($E$9*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>105.9418577407141</v>
+        <v>106.65583399960785</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="11"/>
-        <v>149.82441203991894</v>
+        <v>150.8341269484589</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="11"/>
-        <v>211.8837154814282</v>
+        <v>213.3116679992157</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="11"/>
-        <v>299.64882407983788</v>
+        <v>301.6682538969178</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="11"/>
-        <v>423.76743096285639</v>
+        <v>426.6233359984314</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="11"/>
-        <v>599.29764815967576</v>
+        <v>603.33650779383561</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="11"/>
-        <v>847.53486192571279</v>
+        <v>853.2466719968628</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="11"/>
-        <v>1198.5952963193515</v>
+        <v>1206.6730155876712</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="11"/>
-        <v>1695.0697238514256</v>
+        <v>1706.4933439937256</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="11"/>
-        <v>2397.190592638703</v>
+        <v>2413.3460311753424</v>
       </c>
       <c r="P9" s="5">
         <f t="shared" si="11"/>
-        <v>3390.1394477028512</v>
+        <v>3412.9866879874512</v>
       </c>
       <c r="Q9" s="5">
         <f t="shared" si="11"/>
-        <v>4794.3811852774061</v>
+        <v>4826.6920623506849</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -1120,51 +1125,51 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" ref="F10:Q10" si="12">($E$10*F$5)/SQRT($E$10*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>60.962951667848699</v>
+        <v>61.830921493944608</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="12"/>
-        <v>86.214633050967123</v>
+        <v>87.442127750762566</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="12"/>
-        <v>121.9259033356974</v>
+        <v>123.66184298788922</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="12"/>
-        <v>172.42926610193425</v>
+        <v>174.88425550152513</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="12"/>
-        <v>243.8518066713948</v>
+        <v>247.32368597577843</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="12"/>
-        <v>344.85853220386849</v>
+        <v>349.76851100305026</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="12"/>
-        <v>487.70361334278959</v>
+        <v>494.64737195155686</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="12"/>
-        <v>689.71706440773698</v>
+        <v>699.53702200610053</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="12"/>
-        <v>975.40722668557919</v>
+        <v>989.29474390311373</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="12"/>
-        <v>1379.434128815474</v>
+        <v>1399.0740440122011</v>
       </c>
       <c r="P10" s="5">
         <f t="shared" si="12"/>
-        <v>1950.8144533711584</v>
+        <v>1978.5894878062275</v>
       </c>
       <c r="Q10" s="5">
         <f t="shared" si="12"/>
-        <v>2758.8682576309479</v>
+        <v>2798.1480880244021</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1183,51 +1188,51 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" ref="F11:Q11" si="13">($E$11*F$5)/SQRT($E$11*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>32.249554361531906</v>
+        <v>33.073856000023554</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="13"/>
-        <v>45.60775715856682</v>
+        <v>46.773495715208078</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="13"/>
-        <v>64.499108723063813</v>
+        <v>66.147712000047107</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="13"/>
-        <v>91.215514317133639</v>
+        <v>93.546991430416156</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="13"/>
-        <v>128.99821744612763</v>
+        <v>132.29542400009421</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="13"/>
-        <v>182.43102863426728</v>
+        <v>187.09398286083231</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="13"/>
-        <v>257.99643489225525</v>
+        <v>264.59084800018843</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="13"/>
-        <v>364.86205726853456</v>
+        <v>374.18796572166463</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="13"/>
-        <v>515.9928697845105</v>
+        <v>529.18169600037686</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="13"/>
-        <v>729.72411453706911</v>
+        <v>748.37593144332925</v>
       </c>
       <c r="P11" s="5">
         <f t="shared" si="13"/>
-        <v>1031.985739569021</v>
+        <v>1058.3633920007537</v>
       </c>
       <c r="Q11" s="5">
         <f t="shared" si="13"/>
-        <v>1459.4482290741382</v>
+        <v>1496.7518628866585</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1246,51 +1251,51 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:Q12" si="14">($E$12*F$5)/SQRT($E$12*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>15.398473783546747</v>
+        <v>15.974429754314798</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="14"/>
-        <v>21.776730464538353</v>
+        <v>22.591255209728295</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="14"/>
-        <v>30.796947567093493</v>
+        <v>31.948859508629596</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="14"/>
-        <v>43.553460929076707</v>
+        <v>45.182510419456591</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="14"/>
-        <v>61.593895134186987</v>
+        <v>63.897719017259192</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="14"/>
-        <v>87.106921858153413</v>
+        <v>90.365020838913182</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="14"/>
-        <v>123.18779026837397</v>
+        <v>127.79543803451838</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="14"/>
-        <v>174.21384371630683</v>
+        <v>180.73004167782636</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="14"/>
-        <v>246.37558053674795</v>
+        <v>255.59087606903677</v>
       </c>
       <c r="O12" s="5">
         <f t="shared" si="14"/>
-        <v>348.42768743261365</v>
+        <v>361.46008335565273</v>
       </c>
       <c r="P12" s="5">
         <f t="shared" si="14"/>
-        <v>492.75116107349589</v>
+        <v>511.18175213807353</v>
       </c>
       <c r="Q12" s="5">
         <f t="shared" si="14"/>
-        <v>696.8553748652273</v>
+        <v>722.92016671130546</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1303,51 +1308,51 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13:Q13" si="15">($E$13*F$5)/SQRT($E$13*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>6.747406527050865</v>
+        <v>7.0568798019711805</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="15"/>
-        <v>9.5422738214000784</v>
+        <v>9.9799351239844043</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="15"/>
-        <v>13.49481305410173</v>
+        <v>14.113759603942361</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="15"/>
-        <v>19.084547642800157</v>
+        <v>19.959870247968809</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="15"/>
-        <v>26.98962610820346</v>
+        <v>28.227519207884722</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="15"/>
-        <v>38.169095285600314</v>
+        <v>39.919740495937617</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="15"/>
-        <v>53.97925221640692</v>
+        <v>56.455038415769444</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="15"/>
-        <v>76.338190571200627</v>
+        <v>79.839480991875234</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="15"/>
-        <v>107.95850443281384</v>
+        <v>112.91007683153889</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="15"/>
-        <v>152.67638114240125</v>
+        <v>159.67896198375047</v>
       </c>
       <c r="P13" s="5">
         <f t="shared" si="15"/>
-        <v>215.91700886562768</v>
+        <v>225.82015366307778</v>
       </c>
       <c r="Q13" s="5">
         <f t="shared" si="15"/>
-        <v>305.35276228480251</v>
+        <v>319.35792396750094</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1363,51 +1368,51 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" ref="F14:Q14" si="16">($E$14*F$5)/SQRT($E$14*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>2.8069530996587697</v>
+        <v>2.9484405587011335</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="16"/>
-        <v>3.9696311424826298</v>
+        <v>4.1697246259660492</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="16"/>
-        <v>5.6139061993175394</v>
+        <v>5.8968811174022671</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="16"/>
-        <v>7.9392622849652597</v>
+        <v>8.3394492519320984</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="16"/>
-        <v>11.227812398635079</v>
+        <v>11.793762234804534</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="16"/>
-        <v>15.878524569930519</v>
+        <v>16.678898503864197</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="16"/>
-        <v>22.455624797270158</v>
+        <v>23.587524469609068</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="16"/>
-        <v>31.757049139861039</v>
+        <v>33.357797007728394</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="16"/>
-        <v>44.911249594540315</v>
+        <v>47.175048939218136</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="16"/>
-        <v>63.514098279722077</v>
+        <v>66.715594015456787</v>
       </c>
       <c r="P14" s="5">
         <f t="shared" si="16"/>
-        <v>89.822499189080631</v>
+        <v>94.350097878436273</v>
       </c>
       <c r="Q14" s="5">
         <f t="shared" si="16"/>
-        <v>127.02819655944415</v>
+        <v>133.43118803091357</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1426,51 +1431,51 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" ref="F15:Q15" si="17">($E$15*F$5)/SQRT($E$15*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>1.1384967098490149</v>
+        <v>1.1982385415432433</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="17"/>
-        <v>1.610077487785623</v>
+        <v>1.6945651964086119</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="17"/>
-        <v>2.2769934196980297</v>
+        <v>2.3964770830864865</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="17"/>
-        <v>3.220154975571246</v>
+        <v>3.3891303928172238</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="17"/>
-        <v>4.5539868393960594</v>
+        <v>4.7929541661729731</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="17"/>
-        <v>6.4403099511424919</v>
+        <v>6.7782607856344477</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="17"/>
-        <v>9.1079736787921188</v>
+        <v>9.5859083323459462</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="17"/>
-        <v>12.880619902284984</v>
+        <v>13.556521571268895</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="17"/>
-        <v>18.215947357584238</v>
+        <v>19.171816664691892</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="17"/>
-        <v>25.761239804569968</v>
+        <v>27.113043142537791</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" si="17"/>
-        <v>36.431894715168475</v>
+        <v>38.343633329383785</v>
       </c>
       <c r="Q15" s="5">
         <f t="shared" si="17"/>
-        <v>51.522479609139936</v>
+        <v>54.226086285075581</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1489,51 +1494,51 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:Q16" si="18">($E$16*F$5)/SQRT($E$16*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>0.45671054496554681</v>
+        <v>0.48107411025379643</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="18"/>
-        <v>0.64588624676908357</v>
+        <v>0.68034153122748853</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="18"/>
-        <v>0.91342108993109361</v>
+        <v>0.96214822050759286</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="18"/>
-        <v>1.2917724935381671</v>
+        <v>1.3606830624549771</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="18"/>
-        <v>1.8268421798621872</v>
+        <v>1.9242964410151857</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="18"/>
-        <v>2.5835449870763343</v>
+        <v>2.7213661249099541</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="18"/>
-        <v>3.6536843597243744</v>
+        <v>3.8485928820303714</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="18"/>
-        <v>5.1670899741526686</v>
+        <v>5.4427322498199082</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="18"/>
-        <v>7.3073687194487489</v>
+        <v>7.6971857640607428</v>
       </c>
       <c r="O16" s="5">
         <f t="shared" si="18"/>
-        <v>10.334179948305337</v>
+        <v>10.885464499639816</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" si="18"/>
-        <v>14.614737438897498</v>
+        <v>15.394371528121486</v>
       </c>
       <c r="Q16" s="5">
         <f t="shared" si="18"/>
-        <v>20.668359896610674</v>
+        <v>21.770928999279633</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1552,51 +1557,51 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17:Q17" si="19">($E$17*F$5)/SQRT($E$17*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>0.18237808170498465</v>
+        <v>0.19217192800143526</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="19"/>
-        <v>0.25792155662677779</v>
+        <v>0.27177214688701568</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="19"/>
-        <v>0.3647561634099693</v>
+        <v>0.38434385600287052</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="19"/>
-        <v>0.51584311325355559</v>
+        <v>0.54354429377403135</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="19"/>
-        <v>0.72951232681993861</v>
+        <v>0.76868771200574104</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="19"/>
-        <v>1.0316862265071112</v>
+        <v>1.0870885875480627</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="19"/>
-        <v>1.4590246536398772</v>
+        <v>1.5373754240114821</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="19"/>
-        <v>2.0633724530142223</v>
+        <v>2.1741771750961254</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="19"/>
-        <v>2.9180493072797544</v>
+        <v>3.0747508480229642</v>
       </c>
       <c r="O17" s="5">
         <f t="shared" si="19"/>
-        <v>4.1267449060284447</v>
+        <v>4.3483543501922508</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="19"/>
-        <v>5.8360986145595088</v>
+        <v>6.1495016960459283</v>
       </c>
       <c r="Q17" s="5">
         <f t="shared" si="19"/>
-        <v>8.2534898120568894</v>
+        <v>8.6967087003845016</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1615,51 +1620,51 @@
       </c>
       <c r="F18" s="5">
         <f>($E$18*F$5)/SQRT($E$18*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>7.2695084462262208E-2</v>
+        <v>7.6609238516817127E-2</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" ref="G18:Q18" si="20">($E$18*G$5)/SQRT($E$18*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>0.10280637436438887</v>
+        <v>0.10834182411355807</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="20"/>
-        <v>0.14539016892452442</v>
+        <v>0.15321847703363425</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="20"/>
-        <v>0.20561274872877774</v>
+        <v>0.21668364822711614</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="20"/>
-        <v>0.29078033784904883</v>
+        <v>0.30643695406726851</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="20"/>
-        <v>0.41122549745755549</v>
+        <v>0.43336729645423228</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="20"/>
-        <v>0.58156067569809766</v>
+        <v>0.61287390813453702</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="20"/>
-        <v>0.82245099491511098</v>
+        <v>0.86673459290846455</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="20"/>
-        <v>1.1631213513961953</v>
+        <v>1.225747816269074</v>
       </c>
       <c r="O18" s="5">
         <f t="shared" si="20"/>
-        <v>1.644901989830222</v>
+        <v>1.7334691858169291</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="20"/>
-        <v>2.3262427027923906</v>
+        <v>2.4514956325381481</v>
       </c>
       <c r="Q18" s="5">
         <f t="shared" si="20"/>
-        <v>3.2898039796604439</v>
+        <v>3.4669383716338582</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1678,51 +1683,51 @@
       </c>
       <c r="F19" s="5">
         <f>($E$19*F$5)/SQRT($E$19*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>2.8954586181232402E-2</v>
+        <v>3.0515251557016281E-2</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" ref="G19:Q19" si="21">($E$19*G$5)/SQRT($E$19*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>4.0947968470399464E-2</v>
+        <v>4.3155082611159128E-2</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="21"/>
-        <v>5.7909172362464803E-2</v>
+        <v>6.1030503114032561E-2</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" si="21"/>
-        <v>8.1895936940798927E-2</v>
+        <v>8.6310165222318255E-2</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="21"/>
-        <v>0.11581834472492961</v>
+        <v>0.12206100622806512</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="21"/>
-        <v>0.16379187388159785</v>
+        <v>0.17262033044463651</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="21"/>
-        <v>0.23163668944985921</v>
+        <v>0.24412201245613024</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="21"/>
-        <v>0.32758374776319571</v>
+        <v>0.34524066088927302</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="21"/>
-        <v>0.46327337889971842</v>
+        <v>0.48824402491226049</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="21"/>
-        <v>0.65516749552639142</v>
+        <v>0.69048132177854604</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="21"/>
-        <v>0.92654675779943685</v>
+        <v>0.97648804982452098</v>
       </c>
       <c r="Q19" s="5">
         <f t="shared" si="21"/>
-        <v>1.3103349910527828</v>
+        <v>1.3809626435570921</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1741,51 +1746,51 @@
       </c>
       <c r="F20" s="5">
         <f>($E$20*F$5)/SQRT($E$20*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>1.1529273588403985E-2</v>
+        <v>1.21509687240873E-2</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" ref="G20:Q20" si="22">($E$20*G$5)/SQRT($E$20*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>1.6304855073030835E-2</v>
+        <v>1.7184064765575564E-2</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="22"/>
-        <v>2.305854717680797E-2</v>
+        <v>2.4301937448174601E-2</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" si="22"/>
-        <v>3.260971014606167E-2</v>
+        <v>3.4368129531151127E-2</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="22"/>
-        <v>4.6117094353615939E-2</v>
+        <v>4.8603874896349201E-2</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="22"/>
-        <v>6.521942029212334E-2</v>
+        <v>6.8736259062302255E-2</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="22"/>
-        <v>9.2234188707231879E-2</v>
+        <v>9.7207749792698403E-2</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="22"/>
-        <v>0.13043884058424668</v>
+        <v>0.13747251812460451</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="22"/>
-        <v>0.18446837741446376</v>
+        <v>0.19441549958539681</v>
       </c>
       <c r="O20" s="5">
         <f t="shared" si="22"/>
-        <v>0.26087768116849336</v>
+        <v>0.27494503624920902</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="22"/>
-        <v>0.36893675482892752</v>
+        <v>0.38883099917079361</v>
       </c>
       <c r="Q20" s="5">
         <f t="shared" si="22"/>
-        <v>0.52175536233698672</v>
+        <v>0.54989007249841804</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1798,51 +1803,51 @@
       </c>
       <c r="F21" s="5">
         <f>($E$21*F$5)/SQRT($E$21*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>4.5902424738842353E-3</v>
+        <v>4.8378045196732136E-3</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" ref="G21:Q21" si="23">($E$21*G$5)/SQRT($E$21*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>6.4915831611481135E-3</v>
+        <v>6.841688763831716E-3</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="23"/>
-        <v>9.1804849477684705E-3</v>
+        <v>9.6756090393464271E-3</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="23"/>
-        <v>1.2983166322296227E-2</v>
+        <v>1.3683377527663432E-2</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="23"/>
-        <v>1.8360969895536941E-2</v>
+        <v>1.9351218078692854E-2</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="23"/>
-        <v>2.5966332644592454E-2</v>
+        <v>2.7366755055326864E-2</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="23"/>
-        <v>3.6721939791073882E-2</v>
+        <v>3.8702436157385708E-2</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="23"/>
-        <v>5.1932665289184908E-2</v>
+        <v>5.4733510110653728E-2</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="23"/>
-        <v>7.3443879582147764E-2</v>
+        <v>7.7404872314771417E-2</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="23"/>
-        <v>0.10386533057836982</v>
+        <v>0.10946702022130746</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="23"/>
-        <v>0.14688775916429553</v>
+        <v>0.15480974462954283</v>
       </c>
       <c r="Q21" s="5">
         <f t="shared" si="23"/>
-        <v>0.20773066115673963</v>
+        <v>0.21893404044261491</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1850,7 +1855,7 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
@@ -1868,7 +1873,7 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E23" s="4">
         <f>(((B5*B35)*(B52*B39)^2)/B42) * B11 * B46 * B43 * B48</f>
@@ -1885,10 +1890,10 @@
       <c r="C24" s="2"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="8"/>
+      <c r="A28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
@@ -2033,7 +2038,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="2">
         <v>8.0000000000000002E-3</v>
@@ -2042,13 +2047,13 @@
         <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="2">
         <f>(PI()*B12^2)/4 - B45</f>
@@ -2093,7 +2098,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2118,7 +2123,7 @@
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23 F7:Q21">
+  <conditionalFormatting sqref="F7:Q21 F23">
     <cfRule type="cellIs" dxfId="3" priority="21" operator="greaterThan">
       <formula>$E$3</formula>
     </cfRule>
@@ -2131,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206BC085-F865-5343-9D72-2D200448657F}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2146,16 +2151,16 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -2163,7 +2168,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>5</v>
@@ -2171,7 +2176,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2224,7 +2229,7 @@
         <v>4096</v>
       </c>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -2283,36 +2288,36 @@
         <v>8192</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
@@ -2330,51 +2335,51 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" ref="F7:Q7" si="2">($E$7*F$5)/SQRT($E$7*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>965.8372676281889</v>
+        <v>965.94039802642112</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="2"/>
-        <v>1365.9001629251575</v>
+        <v>1366.0460113330303</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="2"/>
-        <v>1931.6745352563778</v>
+        <v>1931.8807960528422</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="2"/>
-        <v>2731.8003258503149</v>
+        <v>2732.0920226660605</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="2"/>
-        <v>3863.3490705127556</v>
+        <v>3863.7615921056845</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="2"/>
-        <v>5463.6006517006299</v>
+        <v>5464.1840453321211</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="2"/>
-        <v>7726.6981410255112</v>
+        <v>7727.523184211369</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="2"/>
-        <v>10927.20130340126</v>
+        <v>10928.368090664242</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="2"/>
-        <v>15453.396282051022</v>
+        <v>15455.046368422738</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="2"/>
-        <v>21854.40260680252</v>
+        <v>21856.736181328484</v>
       </c>
       <c r="P7" s="5">
         <f t="shared" si="2"/>
-        <v>30906.792564102045</v>
+        <v>30910.092736845476</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="2"/>
-        <v>43708.805213605039</v>
+        <v>43713.472362656968</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -2382,7 +2387,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="1">
         <v>11</v>
@@ -2393,58 +2398,58 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" ref="F8:Q8" si="4">($E$8*F$5)/SQRT($E$8*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>608.92060017097185</v>
+        <v>609.08370308780468</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="4"/>
-        <v>861.14377117015317</v>
+        <v>861.37443352720084</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>1217.8412003419437</v>
+        <v>1218.1674061756094</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="4"/>
-        <v>1722.2875423403063</v>
+        <v>1722.7488670544017</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="4"/>
-        <v>2435.6824006838874</v>
+        <v>2436.3348123512187</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="4"/>
-        <v>3444.5750846806127</v>
+        <v>3445.4977341088033</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="4"/>
-        <v>4871.3648013677748</v>
+        <v>4872.6696247024374</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="4"/>
-        <v>6889.1501693612254</v>
+        <v>6890.9954682176067</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="4"/>
-        <v>9742.7296027355496</v>
+        <v>9745.3392494048749</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="4"/>
-        <v>13778.300338722451</v>
+        <v>13781.990936435213</v>
       </c>
       <c r="P8" s="5">
         <f t="shared" si="4"/>
-        <v>19485.459205471099</v>
+        <v>19490.67849880975</v>
       </c>
       <c r="Q8" s="5">
         <f t="shared" si="4"/>
-        <v>27556.600677444902</v>
+        <v>27563.981872870427</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D9" s="1">
@@ -2456,58 +2461,58 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" ref="F9:Q9" si="5">($E$9*F$5)/SQRT($E$9*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>383.44293643465653</v>
+        <v>383.70006134521583</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="5"/>
-        <v>542.27020110205592</v>
+        <v>542.6338306377927</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="5"/>
-        <v>766.88587286931306</v>
+        <v>767.40012269043166</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>1084.5404022041118</v>
+        <v>1085.2676612755854</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="5"/>
-        <v>1533.7717457386261</v>
+        <v>1534.8002453808633</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="5"/>
-        <v>2169.0808044082237</v>
+        <v>2170.5353225511708</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="5"/>
-        <v>3067.5434914772522</v>
+        <v>3069.6004907617266</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>4338.1616088164474</v>
+        <v>4341.0706451023416</v>
       </c>
       <c r="N9" s="5">
         <f t="shared" si="5"/>
-        <v>6135.0869829545045</v>
+        <v>6139.2009815234533</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="5"/>
-        <v>8676.3232176328947</v>
+        <v>8682.1412902046832</v>
       </c>
       <c r="P9" s="5">
         <f t="shared" si="5"/>
-        <v>12270.173965909009</v>
+        <v>12278.401963046907</v>
       </c>
       <c r="Q9" s="5">
         <f t="shared" si="5"/>
-        <v>17352.646435265789</v>
+        <v>17364.282580409366</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>24576</v>
       </c>
       <c r="D10" s="1">
@@ -2519,51 +2524,51 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" ref="F10:Q10" si="6">($E$10*F$5)/SQRT($E$10*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>240.74407644059974</v>
+        <v>241.14619966773898</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="6"/>
-        <v>340.46353796328128</v>
+        <v>341.0322260848468</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="6"/>
-        <v>481.48815288119948</v>
+        <v>482.29239933547797</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="6"/>
-        <v>680.92707592656257</v>
+        <v>682.0644521696936</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>962.97630576239897</v>
+        <v>964.58479867095593</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="6"/>
-        <v>1361.8541518531251</v>
+        <v>1364.1289043393872</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="6"/>
-        <v>1925.9526115247979</v>
+        <v>1929.1695973419119</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="6"/>
-        <v>2723.7083037062503</v>
+        <v>2728.2578086787744</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" si="6"/>
-        <v>3851.9052230495959</v>
+        <v>3858.3391946838237</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="6"/>
-        <v>5447.4166074125005</v>
+        <v>5456.5156173575488</v>
       </c>
       <c r="P10" s="5">
         <f t="shared" si="6"/>
-        <v>7703.8104460991917</v>
+        <v>7716.6783893676475</v>
       </c>
       <c r="Q10" s="5">
         <f t="shared" si="6"/>
-        <v>10894.833214825001</v>
+        <v>10913.031234715098</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -2582,58 +2587,58 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" ref="F11:Q11" si="7">($E$11*F$5)/SQRT($E$11*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>150.05792500961232</v>
+        <v>150.67459498446485</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="7"/>
-        <v>212.21395269015858</v>
+        <v>213.08605573210329</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="7"/>
-        <v>300.11585001922464</v>
+        <v>301.34918996892969</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="7"/>
-        <v>424.42790538031716</v>
+        <v>426.17211146420658</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="7"/>
-        <v>600.23170003844928</v>
+        <v>602.69837993785939</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>848.85581076063431</v>
+        <v>852.34422292841316</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="7"/>
-        <v>1200.4634000768986</v>
+        <v>1205.3967598757188</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="7"/>
-        <v>1697.7116215212686</v>
+        <v>1704.6884458568263</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="7"/>
-        <v>2400.9268001537971</v>
+        <v>2410.7935197514375</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="7"/>
-        <v>3395.4232430425373</v>
+        <v>3409.3768917136526</v>
       </c>
       <c r="P11" s="5">
         <f t="shared" si="7"/>
-        <v>4801.8536003075942</v>
+        <v>4821.5870395028751</v>
       </c>
       <c r="Q11" s="5">
         <f t="shared" si="7"/>
-        <v>6790.8464860850745</v>
+        <v>6818.7537834273053</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="1">
@@ -2645,51 +2650,51 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" ref="F12:Q12" si="8">($E$12*F$5)/SQRT($E$12*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>91.938555871224452</v>
+        <v>92.841075893644742</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="8"/>
-        <v>130.02075261808216</v>
+        <v>131.29710867410222</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="8"/>
-        <v>183.8771117424489</v>
+        <v>185.68215178728948</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="8"/>
-        <v>260.04150523616431</v>
+        <v>262.59421734820444</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="8"/>
-        <v>367.75422348489781</v>
+        <v>371.36430357457897</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="8"/>
-        <v>520.08301047232862</v>
+        <v>525.18843469640888</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>735.50844696979561</v>
+        <v>742.72860714915794</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="8"/>
-        <v>1040.1660209446572</v>
+        <v>1050.3768693928178</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="8"/>
-        <v>1471.0168939395912</v>
+        <v>1485.4572142983159</v>
       </c>
       <c r="O12" s="5">
         <f t="shared" si="8"/>
-        <v>2080.3320418893145</v>
+        <v>2100.7537387856355</v>
       </c>
       <c r="P12" s="5">
         <f t="shared" si="8"/>
-        <v>2942.0337878791825</v>
+        <v>2970.9144285966318</v>
       </c>
       <c r="Q12" s="5">
         <f t="shared" si="8"/>
-        <v>4160.664083778629</v>
+        <v>4201.507477571271</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -2702,51 +2707,51 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" ref="F13:Q13" si="9">($E$13*F$5)/SQRT($E$13*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>54.250706706882617</v>
+        <v>55.441794223068193</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="9"/>
-        <v>76.722085193198424</v>
+        <v>78.406537312561355</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="9"/>
-        <v>108.50141341376523</v>
+        <v>110.88358844613639</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="9"/>
-        <v>153.44417038639685</v>
+        <v>156.81307462512271</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="9"/>
-        <v>217.00282682753047</v>
+        <v>221.76717689227277</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="9"/>
-        <v>306.8883407727937</v>
+        <v>313.62614925024542</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="9"/>
-        <v>434.00565365506094</v>
+        <v>443.53435378454554</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="9"/>
-        <v>613.77668154558739</v>
+        <v>627.25229850049084</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="9"/>
-        <v>868.01130731012188</v>
+        <v>887.06870756909109</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="9"/>
-        <v>1227.5533630911748</v>
+        <v>1254.5045970009817</v>
       </c>
       <c r="P13" s="5">
         <f t="shared" si="9"/>
-        <v>1736.0226146202438</v>
+        <v>1774.1374151381822</v>
       </c>
       <c r="Q13" s="5">
         <f t="shared" si="9"/>
-        <v>2455.1067261823496</v>
+        <v>2509.0091940019634</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -2762,51 +2767,51 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" ref="F14:Q14" si="10">($E$14*F$5)/SQRT($E$14*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>29.850325472932475</v>
+        <v>31.141360182693607</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="10"/>
-        <v>42.214735125072174</v>
+        <v>44.040533921110786</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="10"/>
-        <v>59.70065094586495</v>
+        <v>62.282720365387213</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="10"/>
-        <v>84.429470250144348</v>
+        <v>88.081067842221572</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="10"/>
-        <v>119.4013018917299</v>
+        <v>124.56544073077443</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="10"/>
-        <v>168.8589405002887</v>
+        <v>176.16213568444314</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="10"/>
-        <v>238.8026037834598</v>
+        <v>249.13088146154885</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="10"/>
-        <v>337.71788100057739</v>
+        <v>352.32427136888629</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="10"/>
-        <v>477.6052075669196</v>
+        <v>498.26176292309771</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="10"/>
-        <v>675.43576200115479</v>
+        <v>704.64854273777257</v>
       </c>
       <c r="P14" s="5">
         <f t="shared" si="10"/>
-        <v>955.21041513383921</v>
+        <v>996.52352584619541</v>
       </c>
       <c r="Q14" s="5">
         <f t="shared" si="10"/>
-        <v>1350.8715240023096</v>
+        <v>1409.2970854755451</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -2825,51 +2830,51 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" ref="F15:Q15" si="11">($E$15*F$5)/SQRT($E$15*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>14.882140210066558</v>
+        <v>15.930996575824832</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="11"/>
-        <v>21.046524522214106</v>
+        <v>22.529831419650815</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="11"/>
-        <v>29.764280420133115</v>
+        <v>31.861993151649664</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="11"/>
-        <v>42.093049044428213</v>
+        <v>45.05966283930163</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="11"/>
-        <v>59.528560840266231</v>
+        <v>63.723986303299327</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="11"/>
-        <v>84.186098088856426</v>
+        <v>90.119325678603261</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="11"/>
-        <v>119.05712168053246</v>
+        <v>127.44797260659865</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="11"/>
-        <v>168.37219617771285</v>
+        <v>180.23865135720652</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="11"/>
-        <v>238.11424336106492</v>
+        <v>254.89594521319731</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="11"/>
-        <v>336.7443923554257</v>
+        <v>360.47730271441304</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" si="11"/>
-        <v>476.22848672212984</v>
+        <v>509.79189042639462</v>
       </c>
       <c r="Q15" s="5">
         <f t="shared" si="11"/>
-        <v>673.48878471085141</v>
+        <v>720.95460542882608</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -2888,51 +2893,51 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" ref="F16:Q16" si="12">($E$16*F$5)/SQRT($E$16*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>6.7354229838665303</v>
+        <v>7.3690457619482119</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="12"/>
-        <v>9.5253265321035077</v>
+        <v>10.42140445829514</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="12"/>
-        <v>13.470845967733061</v>
+        <v>14.738091523896424</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="12"/>
-        <v>19.050653064207015</v>
+        <v>20.842808916590279</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="12"/>
-        <v>26.941691935466121</v>
+        <v>29.476183047792848</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="12"/>
-        <v>38.101306128414031</v>
+        <v>41.685617833180558</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="12"/>
-        <v>53.883383870932242</v>
+        <v>58.952366095585695</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="12"/>
-        <v>76.202612256828061</v>
+        <v>83.371235666361116</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="12"/>
-        <v>107.76676774186448</v>
+        <v>117.90473219117139</v>
       </c>
       <c r="O16" s="5">
         <f t="shared" si="12"/>
-        <v>152.40522451365612</v>
+        <v>166.74247133272223</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" si="12"/>
-        <v>215.53353548372897</v>
+        <v>235.80946438234278</v>
       </c>
       <c r="Q16" s="5">
         <f t="shared" si="12"/>
-        <v>304.81044902731225</v>
+        <v>333.48494266544446</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2951,51 +2956,51 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17:Q17" si="13">($E$17*F$5)/SQRT($E$17*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>2.8525890734053436</v>
+        <v>3.1622463899351909</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="13"/>
-        <v>4.0341701554871374</v>
+        <v>4.4720917322117053</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="13"/>
-        <v>5.7051781468106872</v>
+        <v>6.3244927798703818</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="13"/>
-        <v>8.0683403109742748</v>
+        <v>8.9441834644234106</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="13"/>
-        <v>11.410356293621374</v>
+        <v>12.648985559740764</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="13"/>
-        <v>16.13668062194855</v>
+        <v>17.888366928846821</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="13"/>
-        <v>22.820712587242749</v>
+        <v>25.297971119481527</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" si="13"/>
-        <v>32.273361243897099</v>
+        <v>35.776733857693642</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="13"/>
-        <v>45.641425174485498</v>
+        <v>50.595942238963055</v>
       </c>
       <c r="O17" s="5">
         <f t="shared" si="13"/>
-        <v>64.546722487794199</v>
+        <v>71.553467715387285</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="13"/>
-        <v>91.282850348970996</v>
+        <v>101.19188447792611</v>
       </c>
       <c r="Q17" s="5">
         <f t="shared" si="13"/>
-        <v>129.0934449755884</v>
+        <v>143.10693543077457</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -3014,51 +3019,51 @@
       </c>
       <c r="F18" s="5">
         <f>($E$18*F$5)/SQRT($E$18*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>1.1666426649273542</v>
+        <v>1.3015566208380018</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" ref="G18:Q18" si="14">($E$18*G$5)/SQRT($E$18*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>1.6498818791833545</v>
+        <v>1.8406790253855982</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="14"/>
-        <v>2.3332853298547085</v>
+        <v>2.6031132416760037</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="14"/>
-        <v>3.299763758366709</v>
+        <v>3.6813580507711965</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="14"/>
-        <v>4.666570659709417</v>
+        <v>5.2062264833520073</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="14"/>
-        <v>6.599527516733418</v>
+        <v>7.362716101542393</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="14"/>
-        <v>9.333141319418834</v>
+        <v>10.412452966704015</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="14"/>
-        <v>13.199055033466836</v>
+        <v>14.725432203084786</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="14"/>
-        <v>18.666282638837668</v>
+        <v>20.824905933408029</v>
       </c>
       <c r="O18" s="5">
         <f t="shared" si="14"/>
-        <v>26.398110066933672</v>
+        <v>29.450864406169572</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="14"/>
-        <v>37.332565277675336</v>
+        <v>41.649811866816059</v>
       </c>
       <c r="Q18" s="5">
         <f t="shared" si="14"/>
-        <v>52.796220133867344</v>
+        <v>58.901728812339144</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -3077,51 +3082,51 @@
       </c>
       <c r="F19" s="5">
         <f>($E$19*F$5)/SQRT($E$19*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>0.46965225816029088</v>
+        <v>0.52541446222401889</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" ref="G19:Q19" si="15">($E$19*G$5)/SQRT($E$19*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>0.66418859308943345</v>
+        <v>0.74304825834417387</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="15"/>
-        <v>0.93930451632058176</v>
+        <v>1.0508289244480378</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" si="15"/>
-        <v>1.3283771861788669</v>
+        <v>1.4860965166883477</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="15"/>
-        <v>1.8786090326411635</v>
+        <v>2.1016578488960755</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="15"/>
-        <v>2.6567543723577338</v>
+        <v>2.9721930333766955</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="15"/>
-        <v>3.757218065282327</v>
+        <v>4.2033156977921511</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="15"/>
-        <v>5.3135087447154676</v>
+        <v>5.944386066753391</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="15"/>
-        <v>7.5144361305646541</v>
+        <v>8.4066313955843022</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="15"/>
-        <v>10.627017489430935</v>
+        <v>11.888772133506782</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="15"/>
-        <v>15.028872261129308</v>
+        <v>16.813262791168604</v>
       </c>
       <c r="Q19" s="5">
         <f t="shared" si="15"/>
-        <v>21.254034978861871</v>
+        <v>23.777544267013564</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -3140,51 +3145,51 @@
       </c>
       <c r="F20" s="5">
         <f>($E$20*F$5)/SQRT($E$20*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>0.18781621784002422</v>
+        <v>0.21035541949702655</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" ref="G20:Q20" si="16">($E$20*G$5)/SQRT($E$20*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>0.26561224250298193</v>
+        <v>0.29748748717137669</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="16"/>
-        <v>0.37563243568004845</v>
+        <v>0.42071083899405309</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" si="16"/>
-        <v>0.53122448500596386</v>
+        <v>0.59497497434275337</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="16"/>
-        <v>0.7512648713600969</v>
+        <v>0.84142167798810619</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="16"/>
-        <v>1.0624489700119277</v>
+        <v>1.1899499486855067</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="16"/>
-        <v>1.5025297427201938</v>
+        <v>1.6828433559762124</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="16"/>
-        <v>2.1248979400238555</v>
+        <v>2.3798998973710135</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="16"/>
-        <v>3.0050594854403876</v>
+        <v>3.3656867119524247</v>
       </c>
       <c r="O20" s="5">
         <f t="shared" si="16"/>
-        <v>4.2497958800477109</v>
+        <v>4.759799794742027</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="16"/>
-        <v>6.0101189708807752</v>
+        <v>6.7313734239048495</v>
       </c>
       <c r="Q20" s="5">
         <f t="shared" si="16"/>
-        <v>8.4995917600954218</v>
+        <v>9.5195995894840539</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -3197,51 +3202,51 @@
       </c>
       <c r="F21" s="5">
         <f>($E$21*F$5)/SQRT($E$21*F$5 + $E$23*F$5 + ($B$52*(F$4*($B$7^2)+($B$8*F$5))))</f>
-        <v>7.4906066311703323E-2</v>
+        <v>8.3933917522498638E-2</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" ref="G21:Q21" si="17">($E$21*G$5)/SQRT($E$21*G$5 + $E$23*G$5 + ($B$52*(G$4*($B$7^2)+($B$8*G$5))))</f>
-        <v>0.10593317488202925</v>
+        <v>0.11870048450342233</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="17"/>
-        <v>0.14981213262340665</v>
+        <v>0.16786783504499728</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="17"/>
-        <v>0.21186634976405849</v>
+        <v>0.23740096900684465</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="17"/>
-        <v>0.29962426524681329</v>
+        <v>0.33573567008999455</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="17"/>
-        <v>0.42373269952811699</v>
+        <v>0.47480193801368931</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="17"/>
-        <v>0.59924853049362659</v>
+        <v>0.67147134017998911</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="17"/>
-        <v>0.84746539905623397</v>
+        <v>0.94960387602737861</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="17"/>
-        <v>1.1984970609872532</v>
+        <v>1.3429426803599782</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="17"/>
-        <v>1.6949307981124679</v>
+        <v>1.8992077520547572</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="17"/>
-        <v>2.3969941219745063</v>
+        <v>2.6858853607199564</v>
       </c>
       <c r="Q21" s="5">
         <f t="shared" si="17"/>
-        <v>3.3898615962249359</v>
+        <v>3.7984155041095145</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -3249,7 +3254,7 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
@@ -3267,7 +3272,7 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E23" s="4">
         <f>(((B5*B35)*(B52*B39)^2)/B42) * B11 * B46 * B43 * B48</f>
@@ -3284,10 +3289,10 @@
       <c r="C24" s="2"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="8"/>
+      <c r="A28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
@@ -3434,24 +3439,24 @@
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="11">
+      <c r="A45" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="9">
         <f>B10*B9*1.1</f>
         <v>0.27033600000000008</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="2">
         <f>(PI()*B12^2)/4 - B45</f>
@@ -3496,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -3521,7 +3526,7 @@
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23 F7:Q21">
+  <conditionalFormatting sqref="F7:Q21 F23">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>$E$3</formula>
     </cfRule>

</xml_diff>